<commit_message>
arreglo puertas y tablas
</commit_message>
<xml_diff>
--- a/public/uploads/KPI VentilaciÃ³n.xlsx
+++ b/public/uploads/KPI VentilaciÃ³n.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Contrato info completa\KPI contrtato\KPI Septiembre 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Contrato info completa\KPI contrtato\Octubre 2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="32">
   <si>
     <t>DIAS</t>
   </si>
@@ -50,18 +50,6 @@
     <t>oficina diablo regimiento</t>
   </si>
   <si>
-    <t>sala muestra tte sub 5</t>
-  </si>
-  <si>
-    <t>oficina talleres mecanicos tte-sub 6</t>
-  </si>
-  <si>
-    <t>casino tte-sub -6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oficinas generales tte- sub-6 </t>
-  </si>
-  <si>
     <t>comedores tte-sub-6</t>
   </si>
   <si>
@@ -77,12 +65,6 @@
     <t>ventilador extractor  taller de Martillo tte-sub-5</t>
   </si>
   <si>
-    <t>Taller de Martillo tte sub-5</t>
-  </si>
-  <si>
-    <t>telecomando tte -sub-5</t>
-  </si>
-  <si>
     <t>sala equipo tte-sub-5</t>
   </si>
   <si>
@@ -110,16 +92,37 @@
     <t>Oficina-Pipa- Norte</t>
   </si>
   <si>
-    <t>Extractor Pozo#1 Talleres mecanico tte-sub-5</t>
-  </si>
-  <si>
-    <t>Extractor Pozo#2 Talleres mecanico tte-sub-5</t>
-  </si>
-  <si>
-    <t>Extractor Pozo#3 Talleres mecanico tte-sub-5</t>
-  </si>
-  <si>
     <t>KPI  ventilación 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casino en mantención eléctrica </t>
+  </si>
+  <si>
+    <t>sala muestra Tte. sub 5</t>
+  </si>
+  <si>
+    <t>oficina talleres mecánicos Tte.-sub 6</t>
+  </si>
+  <si>
+    <t>casino Tte.-sub -6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oficinas generales Tte.- sub-6 </t>
+  </si>
+  <si>
+    <t>Taller de Martillo Tte. sub-5</t>
+  </si>
+  <si>
+    <t>telecomando Tte. -sub-5</t>
+  </si>
+  <si>
+    <t>Extractor Pozo#1 Talleres mecánico tte-sub-5</t>
+  </si>
+  <si>
+    <t>Extractor Pozo#2 Talleres mecánico tte-sub-5</t>
+  </si>
+  <si>
+    <t>Extractor Pozo#3 Talleres mecánico tte-sub-5</t>
   </si>
 </sst>
 </file>
@@ -632,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,7 +654,7 @@
     </row>
     <row r="2" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -682,7 +685,7 @@
     </row>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
-        <v>44795</v>
+        <v>44826</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -718,23 +721,23 @@
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
-        <v>44796</v>
+        <v>44827</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="1"/>
@@ -742,10 +745,10 @@
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="1"/>
@@ -753,10 +756,10 @@
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="1"/>
@@ -764,10 +767,10 @@
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="1"/>
@@ -775,23 +778,23 @@
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
-        <v>44797</v>
+        <v>44830</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="1"/>
@@ -799,10 +802,10 @@
     <row r="15" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="1"/>
@@ -810,26 +813,26 @@
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
-        <v>44798</v>
+        <v>44831</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>4</v>
@@ -862,152 +865,152 @@
     <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
-        <v>44799</v>
+        <v>44832</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7">
-        <v>44802</v>
+        <v>44833</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7"/>
       <c r="C29" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="7">
-        <v>44803</v>
+        <v>44834</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
       <c r="C33" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E33" s="4"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="7">
-        <v>44804</v>
+        <v>44837</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>4</v>
@@ -1040,56 +1043,56 @@
     <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="7"/>
       <c r="C38" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="7">
-        <v>44805</v>
+        <v>44838</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
       <c r="C40" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E40" s="4"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="7"/>
       <c r="C41" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="7">
-        <v>44806</v>
+        <v>44839</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" s="4"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="43" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="7"/>
@@ -1114,110 +1117,110 @@
     <row r="45" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="7"/>
       <c r="C45" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E45" s="5"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="7">
-        <v>44809</v>
+        <v>44840</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E46" s="5"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
       <c r="C47" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E47" s="4"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="7"/>
       <c r="C48" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E48" s="4"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="7"/>
       <c r="C49" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E49" s="4"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="7"/>
       <c r="C50" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E50" s="4"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="9">
-        <v>44810</v>
+        <v>44841</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E51" s="4"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="9"/>
       <c r="C52" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E52" s="4"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="9"/>
       <c r="C53" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E53" s="4"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="9"/>
       <c r="C54" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E54" s="4"/>
     </row>
     <row r="55" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="7">
-        <v>44811</v>
+        <v>44845</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>4</v>
@@ -1250,48 +1253,48 @@
     <row r="58" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="7"/>
       <c r="C58" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E58" s="4"/>
     </row>
     <row r="59" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="7">
-        <v>44812</v>
+        <v>44846</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E59" s="4"/>
     </row>
     <row r="60" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="7"/>
       <c r="C60" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E60" s="4"/>
     </row>
     <row r="61" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="7"/>
       <c r="C61" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E61" s="4"/>
     </row>
     <row r="62" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="7">
-        <v>44813</v>
+        <v>44847</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>4</v>
@@ -1326,172 +1329,172 @@
     <row r="65" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="7"/>
       <c r="C65" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="7"/>
       <c r="C66" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E66" s="4"/>
     </row>
     <row r="67" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="7"/>
       <c r="C67" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E67" s="4"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="7">
-        <v>44816</v>
+        <v>44848</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E68" s="4"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="7"/>
       <c r="C69" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E69" s="4"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70" s="7"/>
       <c r="C70" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E70" s="4"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="7"/>
       <c r="C71" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E71" s="4"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="7"/>
       <c r="C72" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E72" s="4"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="7">
-        <v>44817</v>
+        <v>44851</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E73" s="4"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74" s="7"/>
       <c r="C74" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E74" s="4"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B75" s="7"/>
       <c r="C75" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E75" s="4"/>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B76" s="7"/>
       <c r="C76" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E76" s="4"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77" s="7"/>
       <c r="C77" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E77" s="4"/>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B78" s="9">
-        <v>44818</v>
+        <v>44852</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E78" s="4"/>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B79" s="9"/>
       <c r="C79" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E79" s="4"/>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B80" s="9"/>
       <c r="C80" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E80" s="4"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" s="7">
-        <v>44819</v>
+        <v>44853</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>4</v>
@@ -1524,62 +1527,62 @@
     <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B84" s="7"/>
       <c r="C84" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E84" s="4"/>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B85" s="7">
-        <v>44824</v>
+        <v>44854</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E85" s="4"/>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B86" s="7"/>
       <c r="C86" s="6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E86" s="4"/>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87" s="7"/>
       <c r="C87" s="6" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E87" s="4"/>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B88" s="7"/>
       <c r="C88" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E88" s="4"/>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B89" s="7"/>
       <c r="C89" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E89" s="4"/>
     </row>

</xml_diff>